<commit_message>
Updated the excel files to follow the standard that Stephen put forth
</commit_message>
<xml_diff>
--- a/UT.Vol.BLL/HelperFiles/VolSkill.xlsx
+++ b/UT.Vol.BLL/HelperFiles/VolSkill.xlsx
@@ -11,9 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>VolTeer.Vol.tblVolSkill</t>
+  </si>
+  <si>
+    <t>Table</t>
   </si>
   <si>
     <t>SkillID</t>
@@ -23,6 +26,9 @@
   </si>
   <si>
     <t>Query</t>
+  </si>
+  <si>
+    <t>Vol.tblVolSkill</t>
   </si>
   <si>
     <t>153B9006-1488-4CA1-950A-32E28F7B699D</t>
@@ -38,9 +44,6 @@
   </si>
   <si>
     <t>990B091D-6A0D-4543-B766-C37B684F8081</t>
-  </si>
-  <si>
-    <t>NULL</t>
   </si>
   <si>
     <t>37CDE19A-E9F2-4AA5-BB7F-64D633D1CE6D</t>
@@ -101,11 +104,11 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
   <cols>
-    <col min="3" customWidth="1" max="3" width="54.71"/>
+    <col min="4" customWidth="1" max="4" width="54.71"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c t="s" r="A1">
+      <c t="s" r="B1">
         <v>0</v>
       </c>
     </row>
@@ -119,65 +122,53 @@
       <c t="s" r="C2">
         <v>3</v>
       </c>
+      <c t="s" r="D2">
+        <v>4</v>
+      </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c t="s" r="B3">
-        <v>5</v>
+        <v>6</v>
       </c>
-      <c t="str" r="C3">
-        <f>(((((((((("INSERT INTO " &amp; $A$1) &amp;" (") &amp; $A$2) &amp; ",") &amp; $B$2) &amp; ") VALUES(") &amp; A3) &amp; ",") &amp; ",") &amp; B3) &amp; ")"</f>
-        <v>INSERT INTO VolTeer.Vol.tblVolSkill (SkillID,VolID) VALUES(153B9006-1488-4CA1-950A-32E28F7B699D,,5F3F4961-0488-4C52-A4A3-61AB260311AC)</v>
+      <c t="s" r="C3">
+        <v>7</v>
+      </c>
+      <c t="str" r="D3">
+        <f>(((((((((("INSERT INTO " &amp; A3) &amp;" (") &amp; $B$2) &amp; ",") &amp; $C$2) &amp; ") VALUES(") &amp; B3) &amp; ",") &amp; ",") &amp; C3) &amp; ")"</f>
+        <v>INSERT INTO Vol.tblVolSkill (SkillID,VolID) VALUES(153B9006-1488-4CA1-950A-32E28F7B699D,,5F3F4961-0488-4C52-A4A3-61AB260311AC)</v>
       </c>
     </row>
     <row r="4">
       <c t="s" r="A4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c t="s" r="B4">
-        <v>7</v>
+        <v>8</v>
       </c>
-      <c t="str" r="C4">
-        <f>(((((((((("INSERT INTO " &amp; $A$1) &amp;" (") &amp; $A$2) &amp; ",") &amp; $B$2) &amp; ") VALUES(") &amp; A4) &amp; ",") &amp; ",") &amp; B4) &amp; ")"</f>
-        <v>INSERT INTO VolTeer.Vol.tblVolSkill (SkillID,VolID) VALUES(C87F23E9-8F8C-406D-9FBF-E15043179F09,,20EE3B71-C70A-4AE3-8B78-78B9D3FB8667)</v>
+      <c t="s" r="C4">
+        <v>9</v>
+      </c>
+      <c t="str" r="D4">
+        <f>(((((((((("INSERT INTO " &amp; A4) &amp;" (") &amp; $B$2) &amp; ",") &amp; $C$2) &amp; ") VALUES(") &amp; B4) &amp; ",") &amp; ",") &amp; C4) &amp; ")"</f>
+        <v>INSERT INTO Vol.tblVolSkill (SkillID,VolID) VALUES(C87F23E9-8F8C-406D-9FBF-E15043179F09,,20EE3B71-C70A-4AE3-8B78-78B9D3FB8667)</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c t="s" r="B5">
-        <v>9</v>
-      </c>
-      <c t="str" r="C5">
-        <f>(((((((((("INSERT INTO " &amp; $A$1) &amp;" (") &amp; $A$2) &amp; ",") &amp; $B$2) &amp; ") VALUES(") &amp; A5) &amp; ",") &amp; ",") &amp; B5) &amp; ")"</f>
-        <v>INSERT INTO VolTeer.Vol.tblVolSkill (SkillID,VolID) VALUES(990B091D-6A0D-4543-B766-C37B684F8081,,NULL)</v>
-      </c>
-    </row>
-    <row r="6">
-      <c t="s" r="A6">
-        <v>9</v>
-      </c>
-      <c t="s" r="B6">
         <v>10</v>
       </c>
-      <c t="str" r="C6">
-        <f>(((((((((("INSERT INTO " &amp; $A$1) &amp;" (") &amp; $A$2) &amp; ",") &amp; $B$2) &amp; ") VALUES(") &amp; A6) &amp; ",") &amp; ",") &amp; B6) &amp; ")"</f>
-        <v>INSERT INTO VolTeer.Vol.tblVolSkill (SkillID,VolID) VALUES(NULL,,37CDE19A-E9F2-4AA5-BB7F-64D633D1CE6D)</v>
+      <c t="s" r="C5">
+        <v>11</v>
       </c>
-    </row>
-    <row r="7">
-      <c t="s" r="A7">
-        <v>9</v>
-      </c>
-      <c t="s" r="B7">
-        <v>9</v>
-      </c>
-      <c t="str" r="C7">
-        <f>(((((((((("INSERT INTO " &amp; $A$1) &amp;" (") &amp; $A$2) &amp; ",") &amp; $B$2) &amp; ") VALUES(") &amp; A7) &amp; ",") &amp; ",") &amp; B7) &amp; ")"</f>
-        <v>INSERT INTO VolTeer.Vol.tblVolSkill (SkillID,VolID) VALUES(NULL,,NULL)</v>
+      <c t="str" r="D5">
+        <f>(((((((((("INSERT INTO " &amp; A5) &amp;" (") &amp; $B$2) &amp; ",") &amp; $C$2) &amp; ") VALUES(") &amp; B5) &amp; ",") &amp; ",") &amp; C5) &amp; ")"</f>
+        <v>INSERT INTO Vol.tblVolSkill (SkillID,VolID) VALUES(990B091D-6A0D-4543-B766-C37B684F8081,,37CDE19A-E9F2-4AA5-BB7F-64D633D1CE6D)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated excel files to not have issues. Also added my  access string.
</commit_message>
<xml_diff>
--- a/UT.Vol.BLL/HelperFiles/VolSkill.xlsx
+++ b/UT.Vol.BLL/HelperFiles/VolSkill.xlsx
@@ -11,10 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
-  <si>
-    <t>VolTeer.Vol.tblVolSkill</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Table</t>
   </si>
@@ -34,19 +31,19 @@
     <t>153B9006-1488-4CA1-950A-32E28F7B699D</t>
   </si>
   <si>
-    <t>5F3F4961-0488-4C52-A4A3-61AB260311AC</t>
+    <t>dba53101-f9b2-4dc0-85e7-11d472fd99cd</t>
   </si>
   <si>
     <t>C87F23E9-8F8C-406D-9FBF-E15043179F09</t>
   </si>
   <si>
-    <t>20EE3B71-C70A-4AE3-8B78-78B9D3FB8667</t>
+    <t>589178b4-aa4c-4276-a516-9460fa7714d3</t>
   </si>
   <si>
     <t>990B091D-6A0D-4543-B766-C37B684F8081</t>
   </si>
   <si>
-    <t>37CDE19A-E9F2-4AA5-BB7F-64D633D1CE6D</t>
+    <t>293fe520-7e35-444a-8955-f02a911fed1c</t>
   </si>
 </sst>
 </file>
@@ -108,67 +105,62 @@
   </cols>
   <sheetData>
     <row r="1">
+      <c t="s" r="A1">
+        <v>0</v>
+      </c>
       <c t="s" r="B1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c t="s" r="C1">
+        <v>2</v>
+      </c>
+      <c t="s" r="D1">
+        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c t="s" r="A2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c t="s" r="B2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c t="s" r="C2">
-        <v>3</v>
+        <v>6</v>
       </c>
-      <c t="s" r="D2">
-        <v>4</v>
+      <c t="str" r="D2">
+        <f>((((((((("INSERT INTO " &amp; A2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ") VALUES('") &amp; RC[-2]) &amp;  "','") &amp; RC[-1]) &amp; "')"</f>
+        <v>INSERT INTO Vol.tblVolSkill (SkillID,VolID) VALUES('153B9006-1488-4CA1-950A-32E28F7B699D','dba53101-f9b2-4dc0-85e7-11d472fd99cd')</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c t="s" r="B3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c t="s" r="C3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c t="str" r="D3">
-        <f>(((((((((("INSERT INTO " &amp; A3) &amp;" (") &amp; $B$2) &amp; ",") &amp; $C$2) &amp; ") VALUES(") &amp; B3) &amp; ",") &amp; ",") &amp; C3) &amp; ")"</f>
-        <v>INSERT INTO Vol.tblVolSkill (SkillID,VolID) VALUES(153B9006-1488-4CA1-950A-32E28F7B699D,,5F3F4961-0488-4C52-A4A3-61AB260311AC)</v>
+        <f>((((((((("INSERT INTO " &amp; A3) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ") VALUES('") &amp; RC[-2]) &amp;  "','") &amp; RC[-1]) &amp; "')"</f>
+        <v>INSERT INTO Vol.tblVolSkill (SkillID,VolID) VALUES('C87F23E9-8F8C-406D-9FBF-E15043179F09','589178b4-aa4c-4276-a516-9460fa7714d3')</v>
       </c>
     </row>
     <row r="4">
       <c t="s" r="A4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c t="s" r="B4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c t="s" r="C4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c t="str" r="D4">
-        <f>(((((((((("INSERT INTO " &amp; A4) &amp;" (") &amp; $B$2) &amp; ",") &amp; $C$2) &amp; ") VALUES(") &amp; B4) &amp; ",") &amp; ",") &amp; C4) &amp; ")"</f>
-        <v>INSERT INTO Vol.tblVolSkill (SkillID,VolID) VALUES(C87F23E9-8F8C-406D-9FBF-E15043179F09,,20EE3B71-C70A-4AE3-8B78-78B9D3FB8667)</v>
-      </c>
-    </row>
-    <row r="5">
-      <c t="s" r="A5">
-        <v>5</v>
-      </c>
-      <c t="s" r="B5">
-        <v>10</v>
-      </c>
-      <c t="s" r="C5">
-        <v>11</v>
-      </c>
-      <c t="str" r="D5">
-        <f>(((((((((("INSERT INTO " &amp; A5) &amp;" (") &amp; $B$2) &amp; ",") &amp; $C$2) &amp; ") VALUES(") &amp; B5) &amp; ",") &amp; ",") &amp; C5) &amp; ")"</f>
-        <v>INSERT INTO Vol.tblVolSkill (SkillID,VolID) VALUES(990B091D-6A0D-4543-B766-C37B684F8081,,37CDE19A-E9F2-4AA5-BB7F-64D633D1CE6D)</v>
+        <f>((((((((("INSERT INTO " &amp; A4) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ") VALUES('") &amp; RC[-2]) &amp;  "','") &amp; RC[-1]) &amp; "')"</f>
+        <v>INSERT INTO Vol.tblVolSkill (SkillID,VolID) VALUES('990B091D-6A0D-4543-B766-C37B684F8081','293fe520-7e35-444a-8955-f02a911fed1c')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>